<commit_message>
Almost final version of the software coded, missing some trials but overall is almost done. I created one more exception, and finished up a few trial. Documentation was added to the project.
</commit_message>
<xml_diff>
--- a/EscenariosPruebas.xlsx
+++ b/EscenariosPruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\LABS\LAB2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C348049-4D23-4D1A-8982-BCA75D57F95E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7108DB-68CD-49C2-8976-4ECA833CFC58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{1808C89A-E2ED-458B-8C3B-E9683F21B998}"/>
   </bookViews>
@@ -74,12 +74,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -88,7 +103,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>